<commit_message>
Add results and fix the create_excel, I added the creation of subject's performance excel file
</commit_message>
<xml_diff>
--- a/Results_Alpha025/Results_SegRec/Results_Cross/Results_CTNet/seed_results_CTNet.xlsx
+++ b/Results_Alpha025/Results_SegRec/Results_Cross/Results_CTNet/seed_results_CTNet.xlsx
@@ -495,34 +495,34 @@
         <v>42</v>
       </c>
       <c r="B2" t="n">
-        <v>0.772</v>
+        <v>0.77</v>
       </c>
       <c r="C2" t="n">
-        <v>0.714</v>
+        <v>0.71</v>
       </c>
       <c r="D2" t="n">
-        <v>0.759</v>
+        <v>0.76</v>
       </c>
       <c r="E2" t="n">
-        <v>0.972</v>
+        <v>0.97</v>
       </c>
       <c r="F2" t="n">
-        <v>0.912</v>
+        <v>0.91</v>
       </c>
       <c r="G2" t="n">
-        <v>0.869</v>
+        <v>0.87</v>
       </c>
       <c r="H2" t="n">
-        <v>0.909</v>
+        <v>0.91</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>0.884</v>
+        <v>0.88</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8587777777777778</v>
+        <v>0.8577777777777778</v>
       </c>
     </row>
     <row r="3">
@@ -530,34 +530,34 @@
         <v>71</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.696</v>
+        <v>0.7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.772</v>
+        <v>0.77</v>
       </c>
       <c r="E3" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="F3" t="n">
-        <v>0.981</v>
+        <v>0.98</v>
       </c>
       <c r="G3" t="n">
-        <v>0.863</v>
+        <v>0.86</v>
       </c>
       <c r="H3" t="n">
-        <v>0.912</v>
+        <v>0.91</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8644444444444443</v>
+        <v>0.8633333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -565,34 +565,34 @@
         <v>101</v>
       </c>
       <c r="B4" t="n">
-        <v>0.787</v>
+        <v>0.79</v>
       </c>
       <c r="C4" t="n">
-        <v>0.632</v>
+        <v>0.63</v>
       </c>
       <c r="D4" t="n">
-        <v>0.781</v>
+        <v>0.78</v>
       </c>
       <c r="E4" t="n">
-        <v>0.878</v>
+        <v>0.88</v>
       </c>
       <c r="F4" t="n">
-        <v>0.972</v>
+        <v>0.97</v>
       </c>
       <c r="G4" t="n">
-        <v>0.925</v>
+        <v>0.93</v>
       </c>
       <c r="H4" t="n">
-        <v>0.906</v>
+        <v>0.91</v>
       </c>
       <c r="I4" t="n">
-        <v>0.953</v>
+        <v>0.95</v>
       </c>
       <c r="J4" t="n">
-        <v>0.891</v>
+        <v>0.89</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8583333333333334</v>
+        <v>0.8588888888888888</v>
       </c>
     </row>
     <row r="5">
@@ -600,34 +600,34 @@
         <v>113</v>
       </c>
       <c r="B5" t="n">
-        <v>0.791</v>
+        <v>0.79</v>
       </c>
       <c r="C5" t="n">
-        <v>0.711</v>
+        <v>0.71</v>
       </c>
       <c r="D5" t="n">
-        <v>0.769</v>
+        <v>0.77</v>
       </c>
       <c r="E5" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="F5" t="n">
-        <v>0.981</v>
+        <v>0.98</v>
       </c>
       <c r="G5" t="n">
-        <v>0.878</v>
+        <v>0.88</v>
       </c>
       <c r="H5" t="n">
-        <v>0.897</v>
+        <v>0.9</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J5" t="n">
-        <v>0.875</v>
+        <v>0.88</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8606666666666667</v>
+        <v>0.861111111111111</v>
       </c>
     </row>
     <row r="6">
@@ -635,34 +635,34 @@
         <v>127</v>
       </c>
       <c r="B6" t="n">
-        <v>0.753</v>
+        <v>0.75</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>0.744</v>
+        <v>0.74</v>
       </c>
       <c r="E6" t="n">
-        <v>0.859</v>
+        <v>0.86</v>
       </c>
       <c r="F6" t="n">
-        <v>0.969</v>
+        <v>0.97</v>
       </c>
       <c r="G6" t="n">
-        <v>0.872</v>
+        <v>0.87</v>
       </c>
       <c r="H6" t="n">
-        <v>0.919</v>
+        <v>0.92</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>0.894</v>
+        <v>0.89</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8485555555555556</v>
+        <v>0.8477777777777777</v>
       </c>
     </row>
     <row r="7">
@@ -670,34 +670,34 @@
         <v>131</v>
       </c>
       <c r="B7" t="n">
-        <v>0.762</v>
+        <v>0.76</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.791</v>
+        <v>0.79</v>
       </c>
       <c r="E7" t="n">
-        <v>0.931</v>
+        <v>0.93</v>
       </c>
       <c r="F7" t="n">
-        <v>0.991</v>
+        <v>0.99</v>
       </c>
       <c r="G7" t="n">
-        <v>0.866</v>
+        <v>0.87</v>
       </c>
       <c r="H7" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="I7" t="n">
-        <v>0.947</v>
+        <v>0.95</v>
       </c>
       <c r="J7" t="n">
-        <v>0.912</v>
+        <v>0.91</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8657777777777778</v>
+        <v>0.8655555555555555</v>
       </c>
     </row>
     <row r="8">
@@ -705,34 +705,34 @@
         <v>139</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>0.711</v>
+        <v>0.71</v>
       </c>
       <c r="D8" t="n">
         <v>0.8</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9340000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="F8" t="n">
-        <v>0.972</v>
+        <v>0.97</v>
       </c>
       <c r="G8" t="n">
-        <v>0.856</v>
+        <v>0.86</v>
       </c>
       <c r="H8" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="I8" t="n">
-        <v>0.944</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8702222222222223</v>
+        <v>0.8688888888888889</v>
       </c>
     </row>
     <row r="9">
@@ -740,34 +740,34 @@
         <v>149</v>
       </c>
       <c r="B9" t="n">
-        <v>0.766</v>
+        <v>0.77</v>
       </c>
       <c r="C9" t="n">
-        <v>0.725</v>
+        <v>0.72</v>
       </c>
       <c r="D9" t="n">
-        <v>0.719</v>
+        <v>0.72</v>
       </c>
       <c r="E9" t="n">
-        <v>0.963</v>
+        <v>0.96</v>
       </c>
       <c r="F9" t="n">
-        <v>0.972</v>
+        <v>0.97</v>
       </c>
       <c r="G9" t="n">
-        <v>0.884</v>
+        <v>0.88</v>
       </c>
       <c r="H9" t="n">
-        <v>0.906</v>
+        <v>0.91</v>
       </c>
       <c r="I9" t="n">
-        <v>0.947</v>
+        <v>0.95</v>
       </c>
       <c r="J9" t="n">
-        <v>0.891</v>
+        <v>0.89</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8636666666666666</v>
+        <v>0.8633333333333333</v>
       </c>
     </row>
     <row r="10">
@@ -775,34 +775,34 @@
         <v>157</v>
       </c>
       <c r="B10" t="n">
-        <v>0.775</v>
+        <v>0.78</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>0.775</v>
+        <v>0.78</v>
       </c>
       <c r="E10" t="n">
         <v>0.9</v>
       </c>
       <c r="F10" t="n">
-        <v>0.984</v>
+        <v>0.98</v>
       </c>
       <c r="G10" t="n">
-        <v>0.872</v>
+        <v>0.87</v>
       </c>
       <c r="H10" t="n">
-        <v>0.922</v>
+        <v>0.92</v>
       </c>
       <c r="I10" t="n">
-        <v>0.931</v>
+        <v>0.93</v>
       </c>
       <c r="J10" t="n">
-        <v>0.884</v>
+        <v>0.88</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8595555555555556</v>
+        <v>0.8588888888888889</v>
       </c>
     </row>
     <row r="11">
@@ -810,34 +810,34 @@
         <v>163</v>
       </c>
       <c r="B11" t="n">
-        <v>0.759</v>
+        <v>0.76</v>
       </c>
       <c r="C11" t="n">
-        <v>0.668</v>
+        <v>0.67</v>
       </c>
       <c r="D11" t="n">
-        <v>0.769</v>
+        <v>0.77</v>
       </c>
       <c r="E11" t="n">
-        <v>0.966</v>
+        <v>0.97</v>
       </c>
       <c r="F11" t="n">
-        <v>0.972</v>
+        <v>0.97</v>
       </c>
       <c r="G11" t="n">
-        <v>0.853</v>
+        <v>0.85</v>
       </c>
       <c r="H11" t="n">
-        <v>0.912</v>
+        <v>0.91</v>
       </c>
       <c r="I11" t="n">
-        <v>0.953</v>
+        <v>0.95</v>
       </c>
       <c r="J11" t="n">
-        <v>0.897</v>
+        <v>0.9</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8610000000000001</v>
+        <v>0.8611111111111112</v>
       </c>
     </row>
     <row r="12">
@@ -845,34 +845,34 @@
         <v>173</v>
       </c>
       <c r="B12" t="n">
-        <v>0.772</v>
+        <v>0.77</v>
       </c>
       <c r="C12" t="n">
-        <v>0.704</v>
+        <v>0.7</v>
       </c>
       <c r="D12" t="n">
-        <v>0.709</v>
+        <v>0.71</v>
       </c>
       <c r="E12" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="F12" t="n">
-        <v>0.984</v>
+        <v>0.98</v>
       </c>
       <c r="G12" t="n">
-        <v>0.869</v>
+        <v>0.87</v>
       </c>
       <c r="H12" t="n">
-        <v>0.894</v>
+        <v>0.89</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J12" t="n">
-        <v>0.897</v>
+        <v>0.9</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8525555555555555</v>
+        <v>0.8511111111111112</v>
       </c>
     </row>
     <row r="13">
@@ -880,34 +880,34 @@
         <v>181</v>
       </c>
       <c r="B13" t="n">
-        <v>0.734</v>
+        <v>0.73</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D13" t="n">
         <v>0.75</v>
       </c>
       <c r="E13" t="n">
-        <v>0.966</v>
+        <v>0.97</v>
       </c>
       <c r="F13" t="n">
-        <v>0.963</v>
+        <v>0.96</v>
       </c>
       <c r="G13" t="n">
-        <v>0.897</v>
+        <v>0.9</v>
       </c>
       <c r="H13" t="n">
-        <v>0.894</v>
+        <v>0.89</v>
       </c>
       <c r="I13" t="n">
         <v>0.95</v>
       </c>
       <c r="J13" t="n">
-        <v>0.869</v>
+        <v>0.87</v>
       </c>
       <c r="K13" t="n">
-        <v>0.8568888888888888</v>
+        <v>0.8566666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -915,34 +915,34 @@
         <v>322</v>
       </c>
       <c r="B14" t="n">
-        <v>0.756</v>
+        <v>0.76</v>
       </c>
       <c r="C14" t="n">
-        <v>0.618</v>
+        <v>0.62</v>
       </c>
       <c r="D14" t="n">
-        <v>0.762</v>
+        <v>0.76</v>
       </c>
       <c r="E14" t="n">
-        <v>0.912</v>
+        <v>0.91</v>
       </c>
       <c r="F14" t="n">
-        <v>0.963</v>
+        <v>0.96</v>
       </c>
       <c r="G14" t="n">
-        <v>0.887</v>
+        <v>0.89</v>
       </c>
       <c r="H14" t="n">
-        <v>0.906</v>
+        <v>0.91</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J14" t="n">
-        <v>0.894</v>
+        <v>0.89</v>
       </c>
       <c r="K14" t="n">
-        <v>0.8487777777777779</v>
+        <v>0.8488888888888888</v>
       </c>
     </row>
     <row r="15">
@@ -953,31 +953,31 @@
         <v>0.8</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>0.753</v>
+        <v>0.75</v>
       </c>
       <c r="E15" t="n">
-        <v>0.963</v>
+        <v>0.96</v>
       </c>
       <c r="F15" t="n">
-        <v>0.963</v>
+        <v>0.96</v>
       </c>
       <c r="G15" t="n">
-        <v>0.903</v>
+        <v>0.9</v>
       </c>
       <c r="H15" t="n">
-        <v>0.916</v>
+        <v>0.92</v>
       </c>
       <c r="I15" t="n">
-        <v>0.944</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>0.881</v>
+        <v>0.88</v>
       </c>
       <c r="K15" t="n">
-        <v>0.8684444444444445</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="16">
@@ -990,31 +990,31 @@
         <v>0.775</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="D16" t="n">
         <v>0.761</v>
       </c>
       <c r="E16" t="n">
-        <v>0.925</v>
+        <v>0.924</v>
       </c>
       <c r="F16" t="n">
-        <v>0.97</v>
+        <v>0.968</v>
       </c>
       <c r="G16" t="n">
-        <v>0.878</v>
+        <v>0.879</v>
       </c>
       <c r="H16" t="n">
         <v>0.907</v>
       </c>
       <c r="I16" t="n">
-        <v>0.944</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="J16" t="n">
-        <v>0.891</v>
+        <v>0.89</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8598888888888889</v>
+        <v>0.8593333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>